<commit_message>
1.connect server to mysql database
</commit_message>
<xml_diff>
--- a/cmps115_databaseTable.xlsx
+++ b/cmps115_databaseTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artemishuang/Pictures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artemishuang/Documents/projects/cmpe146/cmps115_GAR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4890E0DC-B84B-5748-96EF-6F43DA1A0601}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F24A47-2FAE-EA48-A2BC-398DF9BB247A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{89E30ADC-3F7C-6E4A-86F8-921F1D3165AE}"/>
+    <workbookView xWindow="840" yWindow="2320" windowWidth="14200" windowHeight="15940" xr2:uid="{89E30ADC-3F7C-6E4A-86F8-921F1D3165AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>UserID</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -607,6 +610,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>

</xml_diff>